<commit_message>
push the fixed code
</commit_message>
<xml_diff>
--- a/tests/artifact/script/Mobile-Purchase_SaleOrder.xlsx
+++ b/tests/artifact/script/Mobile-Purchase_SaleOrder.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="888" firstSheet="2" activeTab="1"/>
+    <workbookView windowWidth="18350" windowHeight="6920" tabRatio="888" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -60,7 +60,20 @@
     <definedName name="javaui">'#system'!$N$2:$N$16</definedName>
     <definedName name="browserstack">'#system'!$G$2:$G$7</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -3892,12 +3905,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -4546,16 +4559,16 @@
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -8024,8 +8037,8 @@
   <sheetPr/>
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B6" sqref="$A6:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="15.5" outlineLevelRow="4"/>
@@ -8231,12 +8244,12 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O147"/>
+  <dimension ref="A1:O121"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="A122" sqref="$A122:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
@@ -11405,448 +11418,6 @@
       <c r="N121" s="57"/>
       <c r="O121" s="47"/>
     </row>
-    <row r="122" ht="23" customHeight="1" spans="1:15">
-      <c r="A122" s="30"/>
-      <c r="B122" s="35"/>
-      <c r="C122" s="36"/>
-      <c r="D122" s="37"/>
-      <c r="E122" s="37"/>
-      <c r="F122" s="37"/>
-      <c r="G122" s="37"/>
-      <c r="H122" s="37"/>
-      <c r="I122" s="37"/>
-      <c r="J122" s="56"/>
-      <c r="K122" s="47"/>
-      <c r="L122" s="57"/>
-      <c r="M122" s="58"/>
-      <c r="N122" s="57"/>
-      <c r="O122" s="47"/>
-    </row>
-    <row r="123" ht="23" customHeight="1" spans="1:15">
-      <c r="A123" s="30"/>
-      <c r="B123" s="35"/>
-      <c r="C123" s="36"/>
-      <c r="D123" s="37"/>
-      <c r="E123" s="37"/>
-      <c r="F123" s="37"/>
-      <c r="G123" s="37"/>
-      <c r="H123" s="37"/>
-      <c r="I123" s="37"/>
-      <c r="J123" s="56"/>
-      <c r="K123" s="47"/>
-      <c r="L123" s="57"/>
-      <c r="M123" s="58"/>
-      <c r="N123" s="57"/>
-      <c r="O123" s="47"/>
-    </row>
-    <row r="124" ht="23" customHeight="1" spans="1:15">
-      <c r="A124" s="30"/>
-      <c r="B124" s="35"/>
-      <c r="C124" s="36"/>
-      <c r="D124" s="37"/>
-      <c r="E124" s="37"/>
-      <c r="F124" s="37"/>
-      <c r="G124" s="37"/>
-      <c r="H124" s="37"/>
-      <c r="I124" s="37"/>
-      <c r="J124" s="56"/>
-      <c r="K124" s="47"/>
-      <c r="L124" s="57"/>
-      <c r="M124" s="58"/>
-      <c r="N124" s="57"/>
-      <c r="O124" s="47"/>
-    </row>
-    <row r="125" ht="23" customHeight="1" spans="1:15">
-      <c r="A125" s="30"/>
-      <c r="B125" s="35"/>
-      <c r="C125" s="36"/>
-      <c r="D125" s="37"/>
-      <c r="E125" s="37"/>
-      <c r="F125" s="37"/>
-      <c r="G125" s="37"/>
-      <c r="H125" s="37"/>
-      <c r="I125" s="37"/>
-      <c r="J125" s="56"/>
-      <c r="K125" s="47"/>
-      <c r="L125" s="57"/>
-      <c r="M125" s="58"/>
-      <c r="N125" s="57"/>
-      <c r="O125" s="47"/>
-    </row>
-    <row r="126" ht="23" customHeight="1" spans="1:15">
-      <c r="A126" s="30"/>
-      <c r="B126" s="35"/>
-      <c r="C126" s="36"/>
-      <c r="D126" s="37"/>
-      <c r="E126" s="37"/>
-      <c r="F126" s="37"/>
-      <c r="G126" s="37"/>
-      <c r="H126" s="37"/>
-      <c r="I126" s="37"/>
-      <c r="J126" s="56"/>
-      <c r="K126" s="47"/>
-      <c r="L126" s="57"/>
-      <c r="M126" s="58"/>
-      <c r="N126" s="57"/>
-      <c r="O126" s="47"/>
-    </row>
-    <row r="127" ht="23" customHeight="1" spans="1:15">
-      <c r="A127" s="30"/>
-      <c r="B127" s="35"/>
-      <c r="C127" s="36"/>
-      <c r="D127" s="37"/>
-      <c r="E127" s="37"/>
-      <c r="F127" s="37"/>
-      <c r="G127" s="37"/>
-      <c r="H127" s="37"/>
-      <c r="I127" s="37"/>
-      <c r="J127" s="56"/>
-      <c r="K127" s="47"/>
-      <c r="L127" s="57"/>
-      <c r="M127" s="58"/>
-      <c r="N127" s="57"/>
-      <c r="O127" s="47"/>
-    </row>
-    <row r="128" ht="23" customHeight="1" spans="1:15">
-      <c r="A128" s="30"/>
-      <c r="B128" s="35"/>
-      <c r="C128" s="36"/>
-      <c r="D128" s="37"/>
-      <c r="E128" s="37"/>
-      <c r="F128" s="37"/>
-      <c r="G128" s="37"/>
-      <c r="H128" s="37"/>
-      <c r="I128" s="37"/>
-      <c r="J128" s="56"/>
-      <c r="K128" s="47"/>
-      <c r="L128" s="57"/>
-      <c r="M128" s="58"/>
-      <c r="N128" s="57"/>
-      <c r="O128" s="47"/>
-    </row>
-    <row r="129" ht="23" customHeight="1" spans="1:15">
-      <c r="A129" s="30"/>
-      <c r="B129" s="35"/>
-      <c r="C129" s="36"/>
-      <c r="D129" s="37"/>
-      <c r="E129" s="37"/>
-      <c r="F129" s="37"/>
-      <c r="G129" s="37"/>
-      <c r="H129" s="37"/>
-      <c r="I129" s="37"/>
-      <c r="J129" s="56"/>
-      <c r="K129" s="47"/>
-      <c r="L129" s="57"/>
-      <c r="M129" s="58"/>
-      <c r="N129" s="57"/>
-      <c r="O129" s="47"/>
-    </row>
-    <row r="130" ht="23" customHeight="1" spans="1:15">
-      <c r="A130" s="30"/>
-      <c r="B130" s="35"/>
-      <c r="C130" s="36"/>
-      <c r="D130" s="37"/>
-      <c r="E130" s="37"/>
-      <c r="F130" s="37"/>
-      <c r="G130" s="37"/>
-      <c r="H130" s="37"/>
-      <c r="I130" s="37"/>
-      <c r="J130" s="56"/>
-      <c r="K130" s="47"/>
-      <c r="L130" s="57"/>
-      <c r="M130" s="58"/>
-      <c r="N130" s="57"/>
-      <c r="O130" s="47"/>
-    </row>
-    <row r="131" ht="23" customHeight="1" spans="1:15">
-      <c r="A131" s="30"/>
-      <c r="B131" s="35"/>
-      <c r="C131" s="36"/>
-      <c r="D131" s="37"/>
-      <c r="E131" s="37"/>
-      <c r="F131" s="37"/>
-      <c r="G131" s="37"/>
-      <c r="H131" s="37"/>
-      <c r="I131" s="37"/>
-      <c r="J131" s="56"/>
-      <c r="K131" s="47"/>
-      <c r="L131" s="57"/>
-      <c r="M131" s="58"/>
-      <c r="N131" s="57"/>
-      <c r="O131" s="47"/>
-    </row>
-    <row r="132" ht="23" customHeight="1" spans="1:15">
-      <c r="A132" s="30"/>
-      <c r="B132" s="35"/>
-      <c r="C132" s="36"/>
-      <c r="D132" s="37"/>
-      <c r="E132" s="37"/>
-      <c r="F132" s="37"/>
-      <c r="G132" s="37"/>
-      <c r="H132" s="37"/>
-      <c r="I132" s="37"/>
-      <c r="J132" s="56"/>
-      <c r="K132" s="47"/>
-      <c r="L132" s="57"/>
-      <c r="M132" s="58"/>
-      <c r="N132" s="57"/>
-      <c r="O132" s="47"/>
-    </row>
-    <row r="133" ht="23" customHeight="1" spans="1:15">
-      <c r="A133" s="30"/>
-      <c r="B133" s="35"/>
-      <c r="C133" s="36"/>
-      <c r="D133" s="37"/>
-      <c r="E133" s="37"/>
-      <c r="F133" s="37"/>
-      <c r="G133" s="37"/>
-      <c r="H133" s="37"/>
-      <c r="I133" s="37"/>
-      <c r="J133" s="56"/>
-      <c r="K133" s="47"/>
-      <c r="L133" s="57"/>
-      <c r="M133" s="58"/>
-      <c r="N133" s="57"/>
-      <c r="O133" s="47"/>
-    </row>
-    <row r="134" ht="23" customHeight="1" spans="1:15">
-      <c r="A134" s="30"/>
-      <c r="B134" s="35"/>
-      <c r="C134" s="36"/>
-      <c r="D134" s="37"/>
-      <c r="E134" s="37"/>
-      <c r="F134" s="37"/>
-      <c r="G134" s="37"/>
-      <c r="H134" s="37"/>
-      <c r="I134" s="37"/>
-      <c r="J134" s="56"/>
-      <c r="K134" s="47"/>
-      <c r="L134" s="57"/>
-      <c r="M134" s="58"/>
-      <c r="N134" s="57"/>
-      <c r="O134" s="47"/>
-    </row>
-    <row r="135" ht="23" customHeight="1" spans="1:15">
-      <c r="A135" s="30"/>
-      <c r="B135" s="35"/>
-      <c r="C135" s="36"/>
-      <c r="D135" s="37"/>
-      <c r="E135" s="37"/>
-      <c r="F135" s="37"/>
-      <c r="G135" s="37"/>
-      <c r="H135" s="37"/>
-      <c r="I135" s="37"/>
-      <c r="J135" s="56"/>
-      <c r="K135" s="47"/>
-      <c r="L135" s="57"/>
-      <c r="M135" s="58"/>
-      <c r="N135" s="57"/>
-      <c r="O135" s="47"/>
-    </row>
-    <row r="136" ht="23" customHeight="1" spans="1:15">
-      <c r="A136" s="30"/>
-      <c r="B136" s="35"/>
-      <c r="C136" s="36"/>
-      <c r="D136" s="37"/>
-      <c r="E136" s="37"/>
-      <c r="F136" s="37"/>
-      <c r="G136" s="37"/>
-      <c r="H136" s="37"/>
-      <c r="I136" s="37"/>
-      <c r="J136" s="56"/>
-      <c r="K136" s="47"/>
-      <c r="L136" s="57"/>
-      <c r="M136" s="58"/>
-      <c r="N136" s="57"/>
-      <c r="O136" s="47"/>
-    </row>
-    <row r="137" ht="23" customHeight="1" spans="1:15">
-      <c r="A137" s="30"/>
-      <c r="B137" s="35"/>
-      <c r="C137" s="36"/>
-      <c r="D137" s="37"/>
-      <c r="E137" s="37"/>
-      <c r="F137" s="37"/>
-      <c r="G137" s="37"/>
-      <c r="H137" s="37"/>
-      <c r="I137" s="37"/>
-      <c r="J137" s="56"/>
-      <c r="K137" s="47"/>
-      <c r="L137" s="57"/>
-      <c r="M137" s="58"/>
-      <c r="N137" s="57"/>
-      <c r="O137" s="47"/>
-    </row>
-    <row r="138" ht="23" customHeight="1" spans="1:15">
-      <c r="A138" s="30"/>
-      <c r="B138" s="35"/>
-      <c r="C138" s="36"/>
-      <c r="D138" s="37"/>
-      <c r="E138" s="37"/>
-      <c r="F138" s="37"/>
-      <c r="G138" s="37"/>
-      <c r="H138" s="37"/>
-      <c r="I138" s="37"/>
-      <c r="J138" s="56"/>
-      <c r="K138" s="47"/>
-      <c r="L138" s="57"/>
-      <c r="M138" s="58"/>
-      <c r="N138" s="57"/>
-      <c r="O138" s="47"/>
-    </row>
-    <row r="139" ht="23" customHeight="1" spans="1:15">
-      <c r="A139" s="30"/>
-      <c r="B139" s="35"/>
-      <c r="C139" s="36"/>
-      <c r="D139" s="37"/>
-      <c r="E139" s="37"/>
-      <c r="F139" s="37"/>
-      <c r="G139" s="37"/>
-      <c r="H139" s="37"/>
-      <c r="I139" s="37"/>
-      <c r="J139" s="56"/>
-      <c r="K139" s="47"/>
-      <c r="L139" s="57"/>
-      <c r="M139" s="58"/>
-      <c r="N139" s="57"/>
-      <c r="O139" s="47"/>
-    </row>
-    <row r="140" ht="23" customHeight="1" spans="1:15">
-      <c r="A140" s="30"/>
-      <c r="B140" s="35"/>
-      <c r="C140" s="36"/>
-      <c r="D140" s="37"/>
-      <c r="E140" s="37"/>
-      <c r="F140" s="37"/>
-      <c r="G140" s="37"/>
-      <c r="H140" s="37"/>
-      <c r="I140" s="37"/>
-      <c r="J140" s="56"/>
-      <c r="K140" s="47"/>
-      <c r="L140" s="57"/>
-      <c r="M140" s="58"/>
-      <c r="N140" s="57"/>
-      <c r="O140" s="47"/>
-    </row>
-    <row r="141" ht="23" customHeight="1" spans="1:15">
-      <c r="A141" s="30"/>
-      <c r="B141" s="35"/>
-      <c r="C141" s="36"/>
-      <c r="D141" s="37"/>
-      <c r="E141" s="37"/>
-      <c r="F141" s="37"/>
-      <c r="G141" s="37"/>
-      <c r="H141" s="37"/>
-      <c r="I141" s="37"/>
-      <c r="J141" s="56"/>
-      <c r="K141" s="47"/>
-      <c r="L141" s="57"/>
-      <c r="M141" s="58"/>
-      <c r="N141" s="57"/>
-      <c r="O141" s="47"/>
-    </row>
-    <row r="142" ht="23" customHeight="1" spans="1:15">
-      <c r="A142" s="30"/>
-      <c r="B142" s="35"/>
-      <c r="C142" s="36"/>
-      <c r="D142" s="37"/>
-      <c r="E142" s="37"/>
-      <c r="F142" s="37"/>
-      <c r="G142" s="37"/>
-      <c r="H142" s="37"/>
-      <c r="I142" s="37"/>
-      <c r="J142" s="56"/>
-      <c r="K142" s="47"/>
-      <c r="L142" s="57"/>
-      <c r="M142" s="58"/>
-      <c r="N142" s="57"/>
-      <c r="O142" s="47"/>
-    </row>
-    <row r="143" ht="23" customHeight="1" spans="1:15">
-      <c r="A143" s="30"/>
-      <c r="B143" s="35"/>
-      <c r="C143" s="36"/>
-      <c r="D143" s="37"/>
-      <c r="E143" s="37"/>
-      <c r="F143" s="37"/>
-      <c r="G143" s="37"/>
-      <c r="H143" s="37"/>
-      <c r="I143" s="37"/>
-      <c r="J143" s="56"/>
-      <c r="K143" s="47"/>
-      <c r="L143" s="57"/>
-      <c r="M143" s="58"/>
-      <c r="N143" s="57"/>
-      <c r="O143" s="47"/>
-    </row>
-    <row r="144" ht="23" customHeight="1" spans="1:15">
-      <c r="A144" s="30"/>
-      <c r="B144" s="35"/>
-      <c r="C144" s="36"/>
-      <c r="D144" s="37"/>
-      <c r="E144" s="37"/>
-      <c r="F144" s="37"/>
-      <c r="G144" s="37"/>
-      <c r="H144" s="37"/>
-      <c r="I144" s="37"/>
-      <c r="J144" s="56"/>
-      <c r="K144" s="47"/>
-      <c r="L144" s="57"/>
-      <c r="M144" s="58"/>
-      <c r="N144" s="57"/>
-      <c r="O144" s="47"/>
-    </row>
-    <row r="145" ht="23" customHeight="1" spans="1:15">
-      <c r="A145" s="30"/>
-      <c r="B145" s="35"/>
-      <c r="C145" s="36"/>
-      <c r="D145" s="37"/>
-      <c r="E145" s="37"/>
-      <c r="F145" s="37"/>
-      <c r="G145" s="37"/>
-      <c r="H145" s="37"/>
-      <c r="I145" s="37"/>
-      <c r="J145" s="56"/>
-      <c r="K145" s="47"/>
-      <c r="L145" s="57"/>
-      <c r="M145" s="58"/>
-      <c r="N145" s="57"/>
-      <c r="O145" s="47"/>
-    </row>
-    <row r="146" ht="23" customHeight="1" spans="1:15">
-      <c r="A146" s="30"/>
-      <c r="B146" s="35"/>
-      <c r="C146" s="36"/>
-      <c r="D146" s="37"/>
-      <c r="E146" s="37"/>
-      <c r="F146" s="37"/>
-      <c r="G146" s="37"/>
-      <c r="H146" s="37"/>
-      <c r="I146" s="37"/>
-      <c r="J146" s="56"/>
-      <c r="K146" s="47"/>
-      <c r="L146" s="57"/>
-      <c r="M146" s="58"/>
-      <c r="N146" s="57"/>
-      <c r="O146" s="47"/>
-    </row>
-    <row r="147" ht="23" customHeight="1" spans="1:15">
-      <c r="A147" s="30"/>
-      <c r="B147" s="35"/>
-      <c r="C147" s="36"/>
-      <c r="D147" s="37"/>
-      <c r="E147" s="37"/>
-      <c r="F147" s="37"/>
-      <c r="G147" s="37"/>
-      <c r="H147" s="37"/>
-      <c r="I147" s="37"/>
-      <c r="J147" s="56"/>
-      <c r="K147" s="47"/>
-      <c r="L147" s="57"/>
-      <c r="M147" s="58"/>
-      <c r="N147" s="57"/>
-      <c r="O147" s="47"/>
-    </row>
   </sheetData>
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0"/>
   <mergeCells count="4">
@@ -12438,17 +12009,6 @@
       <formula>LEFT(N99,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N122:N147">
-    <cfRule type="beginsWith" dxfId="2" priority="451" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N122,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="452" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N122,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="453" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N122,LEN("PASS"))="PASS"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="N1 N25:N28 N51:N53 N32 N84:N88 N73:N76">
     <cfRule type="beginsWith" dxfId="2" priority="454" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
@@ -12494,10 +12054,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C12 C13 C33 C34 C35 C38 C41 C42 C43 C44 C45 C47 C48 C49 C50 C51 C52 C53 C54 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C69 C70 C71 C72 C73 C74 C75 C76 C77 C78 C79 C80 C81 C82 C83 C84 C85 C86 C87 C88 C89 C90 C91 C92 C93 C94 C95 C96 C97 C98 C99 C100 C101 C102 C103 C104 C105 C106 C107 C108 C109 C110 C111 C112 C113 C114 C115 C116 C117 C118 C119 C120 C121 C14:C15 C36:C37 C39:C40 C122:C147">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C12 C13 C33 C34 C35 C38 C41 C42 C43 C44 C45 C47 C48 C49 C50 C51 C52 C53 C54 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C69 C70 C71 C72 C73 C74 C75 C76 C77 C78 C79 C80 C81 C82 C83 C84 C85 C86 C87 C88 C89 C90 C91 C92 C93 C94 C95 C96 C97 C98 C99 C100 C101 C102 C103 C104 C105 C106 C107 C108 C109 C110 C111 C112 C113 C114 C115 C116 C117 C118 C119 C120 C121 C14:C15 C36:C37 C39:C40">
       <formula1>target</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D8 D9 D10 D11 D12 D13 D18 D33 D34 D35 D38 D43 D44 D45 D47 D48 D49 D50 D51 D52 D53 D54 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D71 D72 D73 D74 D75 D76 D77 D78 D79 D80 D81 D82 D83 D84 D85 D86 D87 D88 D89 D90 D91 D92 D93 D94 D95 D96 D97 D98 D99 D100 D101 D102 D103 D104 D105 D106 D107 D108 D109 D110 D111 D112 D113 D114 D115 D116 D117 D118 D119 D120 D121 D14:D15 D36:D37 D39:D40 D41:D42 D122:D147">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D8 D9 D10 D11 D12 D13 D18 D33 D34 D35 D38 D43 D44 D45 D47 D48 D49 D50 D51 D52 D53 D54 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D71 D72 D73 D74 D75 D76 D77 D78 D79 D80 D81 D82 D83 D84 D85 D86 D87 D88 D89 D90 D91 D92 D93 D94 D95 D96 D97 D98 D99 D100 D101 D102 D103 D104 D105 D106 D107 D108 D109 D110 D111 D112 D113 D114 D115 D116 D117 D118 D119 D120 D121 D14:D15 D36:D37 D39:D40 D41:D42">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>
@@ -12509,12 +12069,12 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O190"/>
+  <dimension ref="A1:O120"/>
   <sheetViews>
     <sheetView zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="A121" sqref="$A121:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
@@ -15656,1196 +15216,6 @@
       <c r="N120" s="57"/>
       <c r="O120" s="47"/>
     </row>
-    <row r="121" ht="23" customHeight="1" spans="1:15">
-      <c r="A121" s="30"/>
-      <c r="B121" s="35"/>
-      <c r="C121" s="36"/>
-      <c r="D121" s="37"/>
-      <c r="E121" s="37"/>
-      <c r="F121" s="37"/>
-      <c r="G121" s="37"/>
-      <c r="H121" s="37"/>
-      <c r="I121" s="37"/>
-      <c r="J121" s="56"/>
-      <c r="K121" s="47"/>
-      <c r="L121" s="57"/>
-      <c r="M121" s="58"/>
-      <c r="N121" s="57"/>
-      <c r="O121" s="47"/>
-    </row>
-    <row r="122" ht="23" customHeight="1" spans="1:15">
-      <c r="A122" s="30"/>
-      <c r="B122" s="35"/>
-      <c r="C122" s="36"/>
-      <c r="D122" s="37"/>
-      <c r="E122" s="37"/>
-      <c r="F122" s="37"/>
-      <c r="G122" s="37"/>
-      <c r="H122" s="37"/>
-      <c r="I122" s="37"/>
-      <c r="J122" s="56"/>
-      <c r="K122" s="47"/>
-      <c r="L122" s="57"/>
-      <c r="M122" s="58"/>
-      <c r="N122" s="57"/>
-      <c r="O122" s="47"/>
-    </row>
-    <row r="123" ht="23" customHeight="1" spans="1:15">
-      <c r="A123" s="30"/>
-      <c r="B123" s="35"/>
-      <c r="C123" s="36"/>
-      <c r="D123" s="37"/>
-      <c r="E123" s="37"/>
-      <c r="F123" s="37"/>
-      <c r="G123" s="37"/>
-      <c r="H123" s="37"/>
-      <c r="I123" s="37"/>
-      <c r="J123" s="56"/>
-      <c r="K123" s="47"/>
-      <c r="L123" s="57"/>
-      <c r="M123" s="58"/>
-      <c r="N123" s="57"/>
-      <c r="O123" s="47"/>
-    </row>
-    <row r="124" ht="23" customHeight="1" spans="1:15">
-      <c r="A124" s="30"/>
-      <c r="B124" s="35"/>
-      <c r="C124" s="36"/>
-      <c r="D124" s="37"/>
-      <c r="E124" s="37"/>
-      <c r="F124" s="37"/>
-      <c r="G124" s="37"/>
-      <c r="H124" s="37"/>
-      <c r="I124" s="37"/>
-      <c r="J124" s="56"/>
-      <c r="K124" s="47"/>
-      <c r="L124" s="57"/>
-      <c r="M124" s="58"/>
-      <c r="N124" s="57"/>
-      <c r="O124" s="47"/>
-    </row>
-    <row r="125" ht="23" customHeight="1" spans="1:15">
-      <c r="A125" s="30"/>
-      <c r="B125" s="35"/>
-      <c r="C125" s="36"/>
-      <c r="D125" s="37"/>
-      <c r="E125" s="37"/>
-      <c r="F125" s="37"/>
-      <c r="G125" s="37"/>
-      <c r="H125" s="37"/>
-      <c r="I125" s="37"/>
-      <c r="J125" s="56"/>
-      <c r="K125" s="47"/>
-      <c r="L125" s="57"/>
-      <c r="M125" s="58"/>
-      <c r="N125" s="57"/>
-      <c r="O125" s="47"/>
-    </row>
-    <row r="126" ht="23" customHeight="1" spans="1:15">
-      <c r="A126" s="30"/>
-      <c r="B126" s="35"/>
-      <c r="C126" s="36"/>
-      <c r="D126" s="37"/>
-      <c r="E126" s="37"/>
-      <c r="F126" s="37"/>
-      <c r="G126" s="37"/>
-      <c r="H126" s="37"/>
-      <c r="I126" s="37"/>
-      <c r="J126" s="56"/>
-      <c r="K126" s="47"/>
-      <c r="L126" s="57"/>
-      <c r="M126" s="58"/>
-      <c r="N126" s="57"/>
-      <c r="O126" s="47"/>
-    </row>
-    <row r="127" ht="23" customHeight="1" spans="1:15">
-      <c r="A127" s="30"/>
-      <c r="B127" s="35"/>
-      <c r="C127" s="36"/>
-      <c r="D127" s="37"/>
-      <c r="E127" s="37"/>
-      <c r="F127" s="37"/>
-      <c r="G127" s="37"/>
-      <c r="H127" s="37"/>
-      <c r="I127" s="37"/>
-      <c r="J127" s="56"/>
-      <c r="K127" s="47"/>
-      <c r="L127" s="57"/>
-      <c r="M127" s="58"/>
-      <c r="N127" s="57"/>
-      <c r="O127" s="47"/>
-    </row>
-    <row r="128" ht="23" customHeight="1" spans="1:15">
-      <c r="A128" s="30"/>
-      <c r="B128" s="35"/>
-      <c r="C128" s="36"/>
-      <c r="D128" s="37"/>
-      <c r="E128" s="37"/>
-      <c r="F128" s="37"/>
-      <c r="G128" s="37"/>
-      <c r="H128" s="37"/>
-      <c r="I128" s="37"/>
-      <c r="J128" s="56"/>
-      <c r="K128" s="47"/>
-      <c r="L128" s="57"/>
-      <c r="M128" s="58"/>
-      <c r="N128" s="57"/>
-      <c r="O128" s="47"/>
-    </row>
-    <row r="129" ht="23" customHeight="1" spans="1:15">
-      <c r="A129" s="30"/>
-      <c r="B129" s="35"/>
-      <c r="C129" s="36"/>
-      <c r="D129" s="37"/>
-      <c r="E129" s="37"/>
-      <c r="F129" s="37"/>
-      <c r="G129" s="37"/>
-      <c r="H129" s="37"/>
-      <c r="I129" s="37"/>
-      <c r="J129" s="56"/>
-      <c r="K129" s="47"/>
-      <c r="L129" s="57"/>
-      <c r="M129" s="58"/>
-      <c r="N129" s="57"/>
-      <c r="O129" s="47"/>
-    </row>
-    <row r="130" ht="23" customHeight="1" spans="1:15">
-      <c r="A130" s="30"/>
-      <c r="B130" s="35"/>
-      <c r="C130" s="36"/>
-      <c r="D130" s="37"/>
-      <c r="E130" s="37"/>
-      <c r="F130" s="37"/>
-      <c r="G130" s="37"/>
-      <c r="H130" s="37"/>
-      <c r="I130" s="37"/>
-      <c r="J130" s="56"/>
-      <c r="K130" s="47"/>
-      <c r="L130" s="57"/>
-      <c r="M130" s="58"/>
-      <c r="N130" s="57"/>
-      <c r="O130" s="47"/>
-    </row>
-    <row r="131" ht="23" customHeight="1" spans="1:15">
-      <c r="A131" s="30"/>
-      <c r="B131" s="35"/>
-      <c r="C131" s="36"/>
-      <c r="D131" s="37"/>
-      <c r="E131" s="37"/>
-      <c r="F131" s="37"/>
-      <c r="G131" s="37"/>
-      <c r="H131" s="37"/>
-      <c r="I131" s="37"/>
-      <c r="J131" s="56"/>
-      <c r="K131" s="47"/>
-      <c r="L131" s="57"/>
-      <c r="M131" s="58"/>
-      <c r="N131" s="57"/>
-      <c r="O131" s="47"/>
-    </row>
-    <row r="132" ht="23" customHeight="1" spans="1:15">
-      <c r="A132" s="30"/>
-      <c r="B132" s="35"/>
-      <c r="C132" s="36"/>
-      <c r="D132" s="37"/>
-      <c r="E132" s="37"/>
-      <c r="F132" s="37"/>
-      <c r="G132" s="37"/>
-      <c r="H132" s="37"/>
-      <c r="I132" s="37"/>
-      <c r="J132" s="56"/>
-      <c r="K132" s="47"/>
-      <c r="L132" s="57"/>
-      <c r="M132" s="58"/>
-      <c r="N132" s="57"/>
-      <c r="O132" s="47"/>
-    </row>
-    <row r="133" ht="23" customHeight="1" spans="1:15">
-      <c r="A133" s="30"/>
-      <c r="B133" s="35"/>
-      <c r="C133" s="36"/>
-      <c r="D133" s="37"/>
-      <c r="E133" s="37"/>
-      <c r="F133" s="37"/>
-      <c r="G133" s="37"/>
-      <c r="H133" s="37"/>
-      <c r="I133" s="37"/>
-      <c r="J133" s="56"/>
-      <c r="K133" s="47"/>
-      <c r="L133" s="57"/>
-      <c r="M133" s="58"/>
-      <c r="N133" s="57"/>
-      <c r="O133" s="47"/>
-    </row>
-    <row r="134" ht="23" customHeight="1" spans="1:15">
-      <c r="A134" s="30"/>
-      <c r="B134" s="35"/>
-      <c r="C134" s="36"/>
-      <c r="D134" s="37"/>
-      <c r="E134" s="37"/>
-      <c r="F134" s="37"/>
-      <c r="G134" s="37"/>
-      <c r="H134" s="37"/>
-      <c r="I134" s="37"/>
-      <c r="J134" s="56"/>
-      <c r="K134" s="47"/>
-      <c r="L134" s="57"/>
-      <c r="M134" s="58"/>
-      <c r="N134" s="57"/>
-      <c r="O134" s="47"/>
-    </row>
-    <row r="135" ht="23" customHeight="1" spans="1:15">
-      <c r="A135" s="30"/>
-      <c r="B135" s="35"/>
-      <c r="C135" s="36"/>
-      <c r="D135" s="37"/>
-      <c r="E135" s="37"/>
-      <c r="F135" s="37"/>
-      <c r="G135" s="37"/>
-      <c r="H135" s="37"/>
-      <c r="I135" s="37"/>
-      <c r="J135" s="56"/>
-      <c r="K135" s="47"/>
-      <c r="L135" s="57"/>
-      <c r="M135" s="58"/>
-      <c r="N135" s="57"/>
-      <c r="O135" s="47"/>
-    </row>
-    <row r="136" ht="23" customHeight="1" spans="1:15">
-      <c r="A136" s="30"/>
-      <c r="B136" s="35"/>
-      <c r="C136" s="36"/>
-      <c r="D136" s="37"/>
-      <c r="E136" s="37"/>
-      <c r="F136" s="37"/>
-      <c r="G136" s="37"/>
-      <c r="H136" s="37"/>
-      <c r="I136" s="37"/>
-      <c r="J136" s="56"/>
-      <c r="K136" s="47"/>
-      <c r="L136" s="57"/>
-      <c r="M136" s="58"/>
-      <c r="N136" s="57"/>
-      <c r="O136" s="47"/>
-    </row>
-    <row r="137" ht="23" customHeight="1" spans="1:15">
-      <c r="A137" s="30"/>
-      <c r="B137" s="35"/>
-      <c r="C137" s="36"/>
-      <c r="D137" s="37"/>
-      <c r="E137" s="37"/>
-      <c r="F137" s="37"/>
-      <c r="G137" s="37"/>
-      <c r="H137" s="37"/>
-      <c r="I137" s="37"/>
-      <c r="J137" s="56"/>
-      <c r="K137" s="47"/>
-      <c r="L137" s="57"/>
-      <c r="M137" s="58"/>
-      <c r="N137" s="57"/>
-      <c r="O137" s="47"/>
-    </row>
-    <row r="138" ht="23" customHeight="1" spans="1:15">
-      <c r="A138" s="30"/>
-      <c r="B138" s="35"/>
-      <c r="C138" s="36"/>
-      <c r="D138" s="37"/>
-      <c r="E138" s="37"/>
-      <c r="F138" s="37"/>
-      <c r="G138" s="37"/>
-      <c r="H138" s="37"/>
-      <c r="I138" s="37"/>
-      <c r="J138" s="56"/>
-      <c r="K138" s="47"/>
-      <c r="L138" s="57"/>
-      <c r="M138" s="58"/>
-      <c r="N138" s="57"/>
-      <c r="O138" s="47"/>
-    </row>
-    <row r="139" ht="23" customHeight="1" spans="1:15">
-      <c r="A139" s="30"/>
-      <c r="B139" s="35"/>
-      <c r="C139" s="36"/>
-      <c r="D139" s="37"/>
-      <c r="E139" s="37"/>
-      <c r="F139" s="37"/>
-      <c r="G139" s="37"/>
-      <c r="H139" s="37"/>
-      <c r="I139" s="37"/>
-      <c r="J139" s="56"/>
-      <c r="K139" s="47"/>
-      <c r="L139" s="57"/>
-      <c r="M139" s="58"/>
-      <c r="N139" s="57"/>
-      <c r="O139" s="47"/>
-    </row>
-    <row r="140" ht="23" customHeight="1" spans="1:15">
-      <c r="A140" s="30"/>
-      <c r="B140" s="35"/>
-      <c r="C140" s="36"/>
-      <c r="D140" s="37"/>
-      <c r="E140" s="37"/>
-      <c r="F140" s="37"/>
-      <c r="G140" s="37"/>
-      <c r="H140" s="37"/>
-      <c r="I140" s="37"/>
-      <c r="J140" s="56"/>
-      <c r="K140" s="47"/>
-      <c r="L140" s="57"/>
-      <c r="M140" s="58"/>
-      <c r="N140" s="57"/>
-      <c r="O140" s="47"/>
-    </row>
-    <row r="141" ht="23" customHeight="1" spans="1:15">
-      <c r="A141" s="30"/>
-      <c r="B141" s="35"/>
-      <c r="C141" s="36"/>
-      <c r="D141" s="37"/>
-      <c r="E141" s="37"/>
-      <c r="F141" s="37"/>
-      <c r="G141" s="37"/>
-      <c r="H141" s="37"/>
-      <c r="I141" s="37"/>
-      <c r="J141" s="56"/>
-      <c r="K141" s="47"/>
-      <c r="L141" s="57"/>
-      <c r="M141" s="58"/>
-      <c r="N141" s="57"/>
-      <c r="O141" s="47"/>
-    </row>
-    <row r="142" ht="23" customHeight="1" spans="1:15">
-      <c r="A142" s="30"/>
-      <c r="B142" s="35"/>
-      <c r="C142" s="36"/>
-      <c r="D142" s="37"/>
-      <c r="E142" s="37"/>
-      <c r="F142" s="37"/>
-      <c r="G142" s="37"/>
-      <c r="H142" s="37"/>
-      <c r="I142" s="37"/>
-      <c r="J142" s="56"/>
-      <c r="K142" s="47"/>
-      <c r="L142" s="57"/>
-      <c r="M142" s="58"/>
-      <c r="N142" s="57"/>
-      <c r="O142" s="47"/>
-    </row>
-    <row r="143" ht="23" customHeight="1" spans="1:15">
-      <c r="A143" s="30"/>
-      <c r="B143" s="35"/>
-      <c r="C143" s="36"/>
-      <c r="D143" s="37"/>
-      <c r="E143" s="37"/>
-      <c r="F143" s="37"/>
-      <c r="G143" s="37"/>
-      <c r="H143" s="37"/>
-      <c r="I143" s="37"/>
-      <c r="J143" s="56"/>
-      <c r="K143" s="47"/>
-      <c r="L143" s="57"/>
-      <c r="M143" s="58"/>
-      <c r="N143" s="57"/>
-      <c r="O143" s="47"/>
-    </row>
-    <row r="144" ht="23" customHeight="1" spans="1:15">
-      <c r="A144" s="30"/>
-      <c r="B144" s="35"/>
-      <c r="C144" s="36"/>
-      <c r="D144" s="37"/>
-      <c r="E144" s="37"/>
-      <c r="F144" s="37"/>
-      <c r="G144" s="37"/>
-      <c r="H144" s="37"/>
-      <c r="I144" s="37"/>
-      <c r="J144" s="56"/>
-      <c r="K144" s="47"/>
-      <c r="L144" s="57"/>
-      <c r="M144" s="58"/>
-      <c r="N144" s="57"/>
-      <c r="O144" s="47"/>
-    </row>
-    <row r="145" ht="23" customHeight="1" spans="1:15">
-      <c r="A145" s="30"/>
-      <c r="B145" s="35"/>
-      <c r="C145" s="36"/>
-      <c r="D145" s="37"/>
-      <c r="E145" s="37"/>
-      <c r="F145" s="37"/>
-      <c r="G145" s="37"/>
-      <c r="H145" s="37"/>
-      <c r="I145" s="37"/>
-      <c r="J145" s="56"/>
-      <c r="K145" s="47"/>
-      <c r="L145" s="57"/>
-      <c r="M145" s="58"/>
-      <c r="N145" s="57"/>
-      <c r="O145" s="47"/>
-    </row>
-    <row r="146" ht="23" customHeight="1" spans="1:15">
-      <c r="A146" s="30"/>
-      <c r="B146" s="35"/>
-      <c r="C146" s="36"/>
-      <c r="D146" s="37"/>
-      <c r="E146" s="37"/>
-      <c r="F146" s="37"/>
-      <c r="G146" s="37"/>
-      <c r="H146" s="37"/>
-      <c r="I146" s="37"/>
-      <c r="J146" s="56"/>
-      <c r="K146" s="47"/>
-      <c r="L146" s="57"/>
-      <c r="M146" s="58"/>
-      <c r="N146" s="57"/>
-      <c r="O146" s="47"/>
-    </row>
-    <row r="147" ht="23" customHeight="1" spans="1:15">
-      <c r="A147" s="30"/>
-      <c r="B147" s="35"/>
-      <c r="C147" s="36"/>
-      <c r="D147" s="37"/>
-      <c r="E147" s="37"/>
-      <c r="F147" s="37"/>
-      <c r="G147" s="37"/>
-      <c r="H147" s="37"/>
-      <c r="I147" s="37"/>
-      <c r="J147" s="56"/>
-      <c r="K147" s="47"/>
-      <c r="L147" s="57"/>
-      <c r="M147" s="58"/>
-      <c r="N147" s="57"/>
-      <c r="O147" s="47"/>
-    </row>
-    <row r="148" ht="23" customHeight="1" spans="1:15">
-      <c r="A148" s="30"/>
-      <c r="B148" s="35"/>
-      <c r="C148" s="36"/>
-      <c r="D148" s="37"/>
-      <c r="E148" s="37"/>
-      <c r="F148" s="37"/>
-      <c r="G148" s="37"/>
-      <c r="H148" s="37"/>
-      <c r="I148" s="37"/>
-      <c r="J148" s="56"/>
-      <c r="K148" s="47"/>
-      <c r="L148" s="57"/>
-      <c r="M148" s="58"/>
-      <c r="N148" s="57"/>
-      <c r="O148" s="47"/>
-    </row>
-    <row r="149" ht="23" customHeight="1" spans="1:15">
-      <c r="A149" s="30"/>
-      <c r="B149" s="35"/>
-      <c r="C149" s="36"/>
-      <c r="D149" s="37"/>
-      <c r="E149" s="37"/>
-      <c r="F149" s="37"/>
-      <c r="G149" s="37"/>
-      <c r="H149" s="37"/>
-      <c r="I149" s="37"/>
-      <c r="J149" s="56"/>
-      <c r="K149" s="47"/>
-      <c r="L149" s="57"/>
-      <c r="M149" s="58"/>
-      <c r="N149" s="57"/>
-      <c r="O149" s="47"/>
-    </row>
-    <row r="150" ht="23" customHeight="1" spans="1:15">
-      <c r="A150" s="30"/>
-      <c r="B150" s="35"/>
-      <c r="C150" s="36"/>
-      <c r="D150" s="37"/>
-      <c r="E150" s="37"/>
-      <c r="F150" s="37"/>
-      <c r="G150" s="37"/>
-      <c r="H150" s="37"/>
-      <c r="I150" s="37"/>
-      <c r="J150" s="56"/>
-      <c r="K150" s="47"/>
-      <c r="L150" s="57"/>
-      <c r="M150" s="58"/>
-      <c r="N150" s="57"/>
-      <c r="O150" s="47"/>
-    </row>
-    <row r="151" ht="23" customHeight="1" spans="1:15">
-      <c r="A151" s="30"/>
-      <c r="B151" s="35"/>
-      <c r="C151" s="36"/>
-      <c r="D151" s="37"/>
-      <c r="E151" s="37"/>
-      <c r="F151" s="37"/>
-      <c r="G151" s="37"/>
-      <c r="H151" s="37"/>
-      <c r="I151" s="37"/>
-      <c r="J151" s="56"/>
-      <c r="K151" s="47"/>
-      <c r="L151" s="57"/>
-      <c r="M151" s="58"/>
-      <c r="N151" s="57"/>
-      <c r="O151" s="47"/>
-    </row>
-    <row r="152" ht="23" customHeight="1" spans="1:15">
-      <c r="A152" s="30"/>
-      <c r="B152" s="35"/>
-      <c r="C152" s="36"/>
-      <c r="D152" s="37"/>
-      <c r="E152" s="37"/>
-      <c r="F152" s="37"/>
-      <c r="G152" s="37"/>
-      <c r="H152" s="37"/>
-      <c r="I152" s="37"/>
-      <c r="J152" s="56"/>
-      <c r="K152" s="47"/>
-      <c r="L152" s="57"/>
-      <c r="M152" s="58"/>
-      <c r="N152" s="57"/>
-      <c r="O152" s="47"/>
-    </row>
-    <row r="153" ht="23" customHeight="1" spans="1:15">
-      <c r="A153" s="30"/>
-      <c r="B153" s="35"/>
-      <c r="C153" s="36"/>
-      <c r="D153" s="37"/>
-      <c r="E153" s="37"/>
-      <c r="F153" s="37"/>
-      <c r="G153" s="37"/>
-      <c r="H153" s="37"/>
-      <c r="I153" s="37"/>
-      <c r="J153" s="56"/>
-      <c r="K153" s="47"/>
-      <c r="L153" s="57"/>
-      <c r="M153" s="58"/>
-      <c r="N153" s="57"/>
-      <c r="O153" s="47"/>
-    </row>
-    <row r="154" ht="23" customHeight="1" spans="1:15">
-      <c r="A154" s="30"/>
-      <c r="B154" s="35"/>
-      <c r="C154" s="36"/>
-      <c r="D154" s="37"/>
-      <c r="E154" s="37"/>
-      <c r="F154" s="37"/>
-      <c r="G154" s="37"/>
-      <c r="H154" s="37"/>
-      <c r="I154" s="37"/>
-      <c r="J154" s="56"/>
-      <c r="K154" s="47"/>
-      <c r="L154" s="57"/>
-      <c r="M154" s="58"/>
-      <c r="N154" s="57"/>
-      <c r="O154" s="47"/>
-    </row>
-    <row r="155" ht="23" customHeight="1" spans="1:15">
-      <c r="A155" s="30"/>
-      <c r="B155" s="35"/>
-      <c r="C155" s="36"/>
-      <c r="D155" s="37"/>
-      <c r="E155" s="37"/>
-      <c r="F155" s="37"/>
-      <c r="G155" s="37"/>
-      <c r="H155" s="37"/>
-      <c r="I155" s="37"/>
-      <c r="J155" s="56"/>
-      <c r="K155" s="47"/>
-      <c r="L155" s="57"/>
-      <c r="M155" s="58"/>
-      <c r="N155" s="57"/>
-      <c r="O155" s="47"/>
-    </row>
-    <row r="156" ht="23" customHeight="1" spans="1:15">
-      <c r="A156" s="30"/>
-      <c r="B156" s="35"/>
-      <c r="C156" s="36"/>
-      <c r="D156" s="37"/>
-      <c r="E156" s="37"/>
-      <c r="F156" s="37"/>
-      <c r="G156" s="37"/>
-      <c r="H156" s="37"/>
-      <c r="I156" s="37"/>
-      <c r="J156" s="56"/>
-      <c r="K156" s="47"/>
-      <c r="L156" s="57"/>
-      <c r="M156" s="58"/>
-      <c r="N156" s="57"/>
-      <c r="O156" s="47"/>
-    </row>
-    <row r="157" ht="23" customHeight="1" spans="1:15">
-      <c r="A157" s="30"/>
-      <c r="B157" s="35"/>
-      <c r="C157" s="36"/>
-      <c r="D157" s="37"/>
-      <c r="E157" s="37"/>
-      <c r="F157" s="37"/>
-      <c r="G157" s="37"/>
-      <c r="H157" s="37"/>
-      <c r="I157" s="37"/>
-      <c r="J157" s="56"/>
-      <c r="K157" s="47"/>
-      <c r="L157" s="57"/>
-      <c r="M157" s="58"/>
-      <c r="N157" s="57"/>
-      <c r="O157" s="47"/>
-    </row>
-    <row r="158" ht="23" customHeight="1" spans="1:15">
-      <c r="A158" s="30"/>
-      <c r="B158" s="35"/>
-      <c r="C158" s="36"/>
-      <c r="D158" s="37"/>
-      <c r="E158" s="37"/>
-      <c r="F158" s="37"/>
-      <c r="G158" s="37"/>
-      <c r="H158" s="37"/>
-      <c r="I158" s="37"/>
-      <c r="J158" s="56"/>
-      <c r="K158" s="47"/>
-      <c r="L158" s="57"/>
-      <c r="M158" s="58"/>
-      <c r="N158" s="57"/>
-      <c r="O158" s="47"/>
-    </row>
-    <row r="159" ht="23" customHeight="1" spans="1:15">
-      <c r="A159" s="30"/>
-      <c r="B159" s="35"/>
-      <c r="C159" s="36"/>
-      <c r="D159" s="37"/>
-      <c r="E159" s="37"/>
-      <c r="F159" s="37"/>
-      <c r="G159" s="37"/>
-      <c r="H159" s="37"/>
-      <c r="I159" s="37"/>
-      <c r="J159" s="56"/>
-      <c r="K159" s="47"/>
-      <c r="L159" s="57"/>
-      <c r="M159" s="58"/>
-      <c r="N159" s="57"/>
-      <c r="O159" s="47"/>
-    </row>
-    <row r="160" ht="23" customHeight="1" spans="1:15">
-      <c r="A160" s="30"/>
-      <c r="B160" s="35"/>
-      <c r="C160" s="36"/>
-      <c r="D160" s="37"/>
-      <c r="E160" s="37"/>
-      <c r="F160" s="37"/>
-      <c r="G160" s="37"/>
-      <c r="H160" s="37"/>
-      <c r="I160" s="37"/>
-      <c r="J160" s="56"/>
-      <c r="K160" s="47"/>
-      <c r="L160" s="57"/>
-      <c r="M160" s="58"/>
-      <c r="N160" s="57"/>
-      <c r="O160" s="47"/>
-    </row>
-    <row r="161" ht="23" customHeight="1" spans="1:15">
-      <c r="A161" s="30"/>
-      <c r="B161" s="35"/>
-      <c r="C161" s="36"/>
-      <c r="D161" s="37"/>
-      <c r="E161" s="37"/>
-      <c r="F161" s="37"/>
-      <c r="G161" s="37"/>
-      <c r="H161" s="37"/>
-      <c r="I161" s="37"/>
-      <c r="J161" s="56"/>
-      <c r="K161" s="47"/>
-      <c r="L161" s="57"/>
-      <c r="M161" s="58"/>
-      <c r="N161" s="57"/>
-      <c r="O161" s="47"/>
-    </row>
-    <row r="162" ht="23" customHeight="1" spans="1:15">
-      <c r="A162" s="30"/>
-      <c r="B162" s="35"/>
-      <c r="C162" s="36"/>
-      <c r="D162" s="37"/>
-      <c r="E162" s="37"/>
-      <c r="F162" s="37"/>
-      <c r="G162" s="37"/>
-      <c r="H162" s="37"/>
-      <c r="I162" s="37"/>
-      <c r="J162" s="56"/>
-      <c r="K162" s="47"/>
-      <c r="L162" s="57"/>
-      <c r="M162" s="58"/>
-      <c r="N162" s="57"/>
-      <c r="O162" s="47"/>
-    </row>
-    <row r="163" ht="23" customHeight="1" spans="1:15">
-      <c r="A163" s="30"/>
-      <c r="B163" s="35"/>
-      <c r="C163" s="36"/>
-      <c r="D163" s="37"/>
-      <c r="E163" s="37"/>
-      <c r="F163" s="37"/>
-      <c r="G163" s="37"/>
-      <c r="H163" s="37"/>
-      <c r="I163" s="37"/>
-      <c r="J163" s="56"/>
-      <c r="K163" s="47"/>
-      <c r="L163" s="57"/>
-      <c r="M163" s="58"/>
-      <c r="N163" s="57"/>
-      <c r="O163" s="47"/>
-    </row>
-    <row r="164" ht="23" customHeight="1" spans="1:15">
-      <c r="A164" s="30"/>
-      <c r="B164" s="35"/>
-      <c r="C164" s="36"/>
-      <c r="D164" s="37"/>
-      <c r="E164" s="37"/>
-      <c r="F164" s="37"/>
-      <c r="G164" s="37"/>
-      <c r="H164" s="37"/>
-      <c r="I164" s="37"/>
-      <c r="J164" s="56"/>
-      <c r="K164" s="47"/>
-      <c r="L164" s="57"/>
-      <c r="M164" s="58"/>
-      <c r="N164" s="57"/>
-      <c r="O164" s="47"/>
-    </row>
-    <row r="165" ht="23" customHeight="1" spans="1:15">
-      <c r="A165" s="30"/>
-      <c r="B165" s="35"/>
-      <c r="C165" s="36"/>
-      <c r="D165" s="37"/>
-      <c r="E165" s="37"/>
-      <c r="F165" s="37"/>
-      <c r="G165" s="37"/>
-      <c r="H165" s="37"/>
-      <c r="I165" s="37"/>
-      <c r="J165" s="56"/>
-      <c r="K165" s="47"/>
-      <c r="L165" s="57"/>
-      <c r="M165" s="58"/>
-      <c r="N165" s="57"/>
-      <c r="O165" s="47"/>
-    </row>
-    <row r="166" ht="23" customHeight="1" spans="1:15">
-      <c r="A166" s="30"/>
-      <c r="B166" s="35"/>
-      <c r="C166" s="36"/>
-      <c r="D166" s="37"/>
-      <c r="E166" s="37"/>
-      <c r="F166" s="37"/>
-      <c r="G166" s="37"/>
-      <c r="H166" s="37"/>
-      <c r="I166" s="37"/>
-      <c r="J166" s="56"/>
-      <c r="K166" s="47"/>
-      <c r="L166" s="57"/>
-      <c r="M166" s="58"/>
-      <c r="N166" s="57"/>
-      <c r="O166" s="47"/>
-    </row>
-    <row r="167" ht="23" customHeight="1" spans="1:15">
-      <c r="A167" s="30"/>
-      <c r="B167" s="35"/>
-      <c r="C167" s="36"/>
-      <c r="D167" s="37"/>
-      <c r="E167" s="37"/>
-      <c r="F167" s="37"/>
-      <c r="G167" s="37"/>
-      <c r="H167" s="37"/>
-      <c r="I167" s="37"/>
-      <c r="J167" s="56"/>
-      <c r="K167" s="47"/>
-      <c r="L167" s="57"/>
-      <c r="M167" s="58"/>
-      <c r="N167" s="57"/>
-      <c r="O167" s="47"/>
-    </row>
-    <row r="168" ht="23" customHeight="1" spans="1:15">
-      <c r="A168" s="30"/>
-      <c r="B168" s="35"/>
-      <c r="C168" s="36"/>
-      <c r="D168" s="37"/>
-      <c r="E168" s="37"/>
-      <c r="F168" s="37"/>
-      <c r="G168" s="37"/>
-      <c r="H168" s="37"/>
-      <c r="I168" s="37"/>
-      <c r="J168" s="56"/>
-      <c r="K168" s="47"/>
-      <c r="L168" s="57"/>
-      <c r="M168" s="58"/>
-      <c r="N168" s="57"/>
-      <c r="O168" s="47"/>
-    </row>
-    <row r="169" ht="23" customHeight="1" spans="1:15">
-      <c r="A169" s="30"/>
-      <c r="B169" s="35"/>
-      <c r="C169" s="36"/>
-      <c r="D169" s="37"/>
-      <c r="E169" s="37"/>
-      <c r="F169" s="37"/>
-      <c r="G169" s="37"/>
-      <c r="H169" s="37"/>
-      <c r="I169" s="37"/>
-      <c r="J169" s="56"/>
-      <c r="K169" s="47"/>
-      <c r="L169" s="57"/>
-      <c r="M169" s="58"/>
-      <c r="N169" s="57"/>
-      <c r="O169" s="47"/>
-    </row>
-    <row r="170" ht="23" customHeight="1" spans="1:15">
-      <c r="A170" s="30"/>
-      <c r="B170" s="35"/>
-      <c r="C170" s="36"/>
-      <c r="D170" s="37"/>
-      <c r="E170" s="37"/>
-      <c r="F170" s="37"/>
-      <c r="G170" s="37"/>
-      <c r="H170" s="37"/>
-      <c r="I170" s="37"/>
-      <c r="J170" s="56"/>
-      <c r="K170" s="47"/>
-      <c r="L170" s="57"/>
-      <c r="M170" s="58"/>
-      <c r="N170" s="57"/>
-      <c r="O170" s="47"/>
-    </row>
-    <row r="171" ht="23" customHeight="1" spans="1:15">
-      <c r="A171" s="30"/>
-      <c r="B171" s="35"/>
-      <c r="C171" s="36"/>
-      <c r="D171" s="37"/>
-      <c r="E171" s="37"/>
-      <c r="F171" s="37"/>
-      <c r="G171" s="37"/>
-      <c r="H171" s="37"/>
-      <c r="I171" s="37"/>
-      <c r="J171" s="56"/>
-      <c r="K171" s="47"/>
-      <c r="L171" s="57"/>
-      <c r="M171" s="58"/>
-      <c r="N171" s="57"/>
-      <c r="O171" s="47"/>
-    </row>
-    <row r="172" ht="23" customHeight="1" spans="1:15">
-      <c r="A172" s="30"/>
-      <c r="B172" s="35"/>
-      <c r="C172" s="36"/>
-      <c r="D172" s="37"/>
-      <c r="E172" s="37"/>
-      <c r="F172" s="37"/>
-      <c r="G172" s="37"/>
-      <c r="H172" s="37"/>
-      <c r="I172" s="37"/>
-      <c r="J172" s="56"/>
-      <c r="K172" s="47"/>
-      <c r="L172" s="57"/>
-      <c r="M172" s="58"/>
-      <c r="N172" s="57"/>
-      <c r="O172" s="47"/>
-    </row>
-    <row r="173" ht="23" customHeight="1" spans="1:15">
-      <c r="A173" s="30"/>
-      <c r="B173" s="35"/>
-      <c r="C173" s="36"/>
-      <c r="D173" s="37"/>
-      <c r="E173" s="37"/>
-      <c r="F173" s="37"/>
-      <c r="G173" s="37"/>
-      <c r="H173" s="37"/>
-      <c r="I173" s="37"/>
-      <c r="J173" s="56"/>
-      <c r="K173" s="47"/>
-      <c r="L173" s="57"/>
-      <c r="M173" s="58"/>
-      <c r="N173" s="57"/>
-      <c r="O173" s="47"/>
-    </row>
-    <row r="174" ht="23" customHeight="1" spans="1:15">
-      <c r="A174" s="30"/>
-      <c r="B174" s="35"/>
-      <c r="C174" s="36"/>
-      <c r="D174" s="37"/>
-      <c r="E174" s="37"/>
-      <c r="F174" s="37"/>
-      <c r="G174" s="37"/>
-      <c r="H174" s="37"/>
-      <c r="I174" s="37"/>
-      <c r="J174" s="56"/>
-      <c r="K174" s="47"/>
-      <c r="L174" s="57"/>
-      <c r="M174" s="58"/>
-      <c r="N174" s="57"/>
-      <c r="O174" s="47"/>
-    </row>
-    <row r="175" ht="23" customHeight="1" spans="1:15">
-      <c r="A175" s="30"/>
-      <c r="B175" s="35"/>
-      <c r="C175" s="36"/>
-      <c r="D175" s="37"/>
-      <c r="E175" s="37"/>
-      <c r="F175" s="37"/>
-      <c r="G175" s="37"/>
-      <c r="H175" s="37"/>
-      <c r="I175" s="37"/>
-      <c r="J175" s="56"/>
-      <c r="K175" s="47"/>
-      <c r="L175" s="57"/>
-      <c r="M175" s="58"/>
-      <c r="N175" s="57"/>
-      <c r="O175" s="47"/>
-    </row>
-    <row r="176" ht="23" customHeight="1" spans="1:15">
-      <c r="A176" s="30"/>
-      <c r="B176" s="35"/>
-      <c r="C176" s="36"/>
-      <c r="D176" s="37"/>
-      <c r="E176" s="37"/>
-      <c r="F176" s="37"/>
-      <c r="G176" s="37"/>
-      <c r="H176" s="37"/>
-      <c r="I176" s="37"/>
-      <c r="J176" s="56"/>
-      <c r="K176" s="47"/>
-      <c r="L176" s="57"/>
-      <c r="M176" s="58"/>
-      <c r="N176" s="57"/>
-      <c r="O176" s="47"/>
-    </row>
-    <row r="177" ht="23" customHeight="1" spans="1:15">
-      <c r="A177" s="30"/>
-      <c r="B177" s="35"/>
-      <c r="C177" s="36"/>
-      <c r="D177" s="37"/>
-      <c r="E177" s="37"/>
-      <c r="F177" s="37"/>
-      <c r="G177" s="37"/>
-      <c r="H177" s="37"/>
-      <c r="I177" s="37"/>
-      <c r="J177" s="56"/>
-      <c r="K177" s="47"/>
-      <c r="L177" s="57"/>
-      <c r="M177" s="58"/>
-      <c r="N177" s="57"/>
-      <c r="O177" s="47"/>
-    </row>
-    <row r="178" ht="23" customHeight="1" spans="1:15">
-      <c r="A178" s="30"/>
-      <c r="B178" s="35"/>
-      <c r="C178" s="36"/>
-      <c r="D178" s="37"/>
-      <c r="E178" s="37"/>
-      <c r="F178" s="37"/>
-      <c r="G178" s="37"/>
-      <c r="H178" s="37"/>
-      <c r="I178" s="37"/>
-      <c r="J178" s="56"/>
-      <c r="K178" s="47"/>
-      <c r="L178" s="57"/>
-      <c r="M178" s="58"/>
-      <c r="N178" s="57"/>
-      <c r="O178" s="47"/>
-    </row>
-    <row r="179" ht="23" customHeight="1" spans="1:15">
-      <c r="A179" s="30"/>
-      <c r="B179" s="35"/>
-      <c r="C179" s="36"/>
-      <c r="D179" s="37"/>
-      <c r="E179" s="37"/>
-      <c r="F179" s="37"/>
-      <c r="G179" s="37"/>
-      <c r="H179" s="37"/>
-      <c r="I179" s="37"/>
-      <c r="J179" s="56"/>
-      <c r="K179" s="47"/>
-      <c r="L179" s="57"/>
-      <c r="M179" s="58"/>
-      <c r="N179" s="57"/>
-      <c r="O179" s="47"/>
-    </row>
-    <row r="180" ht="23" customHeight="1" spans="1:15">
-      <c r="A180" s="30"/>
-      <c r="B180" s="35"/>
-      <c r="C180" s="36"/>
-      <c r="D180" s="37"/>
-      <c r="E180" s="37"/>
-      <c r="F180" s="37"/>
-      <c r="G180" s="37"/>
-      <c r="H180" s="37"/>
-      <c r="I180" s="37"/>
-      <c r="J180" s="56"/>
-      <c r="K180" s="47"/>
-      <c r="L180" s="57"/>
-      <c r="M180" s="58"/>
-      <c r="N180" s="57"/>
-      <c r="O180" s="47"/>
-    </row>
-    <row r="181" ht="23" customHeight="1" spans="1:15">
-      <c r="A181" s="30"/>
-      <c r="B181" s="35"/>
-      <c r="C181" s="36"/>
-      <c r="D181" s="37"/>
-      <c r="E181" s="37"/>
-      <c r="F181" s="37"/>
-      <c r="G181" s="37"/>
-      <c r="H181" s="37"/>
-      <c r="I181" s="37"/>
-      <c r="J181" s="56"/>
-      <c r="K181" s="47"/>
-      <c r="L181" s="57"/>
-      <c r="M181" s="58"/>
-      <c r="N181" s="57"/>
-      <c r="O181" s="47"/>
-    </row>
-    <row r="182" ht="23" customHeight="1" spans="1:15">
-      <c r="A182" s="30"/>
-      <c r="B182" s="35"/>
-      <c r="C182" s="36"/>
-      <c r="D182" s="37"/>
-      <c r="E182" s="37"/>
-      <c r="F182" s="37"/>
-      <c r="G182" s="37"/>
-      <c r="H182" s="37"/>
-      <c r="I182" s="37"/>
-      <c r="J182" s="56"/>
-      <c r="K182" s="47"/>
-      <c r="L182" s="57"/>
-      <c r="M182" s="58"/>
-      <c r="N182" s="57"/>
-      <c r="O182" s="47"/>
-    </row>
-    <row r="183" ht="23" customHeight="1" spans="1:15">
-      <c r="A183" s="30"/>
-      <c r="B183" s="35"/>
-      <c r="C183" s="36"/>
-      <c r="D183" s="37"/>
-      <c r="E183" s="37"/>
-      <c r="F183" s="37"/>
-      <c r="G183" s="37"/>
-      <c r="H183" s="37"/>
-      <c r="I183" s="37"/>
-      <c r="J183" s="56"/>
-      <c r="K183" s="47"/>
-      <c r="L183" s="57"/>
-      <c r="M183" s="58"/>
-      <c r="N183" s="57"/>
-      <c r="O183" s="47"/>
-    </row>
-    <row r="184" ht="23" customHeight="1" spans="1:15">
-      <c r="A184" s="30"/>
-      <c r="B184" s="35"/>
-      <c r="C184" s="36"/>
-      <c r="D184" s="37"/>
-      <c r="E184" s="37"/>
-      <c r="F184" s="37"/>
-      <c r="G184" s="37"/>
-      <c r="H184" s="37"/>
-      <c r="I184" s="37"/>
-      <c r="J184" s="56"/>
-      <c r="K184" s="47"/>
-      <c r="L184" s="57"/>
-      <c r="M184" s="58"/>
-      <c r="N184" s="57"/>
-      <c r="O184" s="47"/>
-    </row>
-    <row r="185" ht="23" customHeight="1" spans="1:15">
-      <c r="A185" s="30"/>
-      <c r="B185" s="35"/>
-      <c r="C185" s="36"/>
-      <c r="D185" s="37"/>
-      <c r="E185" s="37"/>
-      <c r="F185" s="37"/>
-      <c r="G185" s="37"/>
-      <c r="H185" s="37"/>
-      <c r="I185" s="37"/>
-      <c r="J185" s="56"/>
-      <c r="K185" s="47"/>
-      <c r="L185" s="57"/>
-      <c r="M185" s="58"/>
-      <c r="N185" s="57"/>
-      <c r="O185" s="47"/>
-    </row>
-    <row r="186" ht="23" customHeight="1" spans="1:15">
-      <c r="A186" s="30"/>
-      <c r="B186" s="35"/>
-      <c r="C186" s="36"/>
-      <c r="D186" s="37"/>
-      <c r="E186" s="37"/>
-      <c r="F186" s="37"/>
-      <c r="G186" s="37"/>
-      <c r="H186" s="37"/>
-      <c r="I186" s="37"/>
-      <c r="J186" s="56"/>
-      <c r="K186" s="47"/>
-      <c r="L186" s="57"/>
-      <c r="M186" s="58"/>
-      <c r="N186" s="57"/>
-      <c r="O186" s="47"/>
-    </row>
-    <row r="187" ht="23" customHeight="1" spans="1:15">
-      <c r="A187" s="30"/>
-      <c r="B187" s="35"/>
-      <c r="C187" s="36"/>
-      <c r="D187" s="37"/>
-      <c r="E187" s="37"/>
-      <c r="F187" s="37"/>
-      <c r="G187" s="37"/>
-      <c r="H187" s="37"/>
-      <c r="I187" s="37"/>
-      <c r="J187" s="56"/>
-      <c r="K187" s="47"/>
-      <c r="L187" s="57"/>
-      <c r="M187" s="58"/>
-      <c r="N187" s="57"/>
-      <c r="O187" s="47"/>
-    </row>
-    <row r="188" ht="23" customHeight="1" spans="1:15">
-      <c r="A188" s="30"/>
-      <c r="B188" s="35"/>
-      <c r="C188" s="36"/>
-      <c r="D188" s="37"/>
-      <c r="E188" s="37"/>
-      <c r="F188" s="37"/>
-      <c r="G188" s="37"/>
-      <c r="H188" s="37"/>
-      <c r="I188" s="37"/>
-      <c r="J188" s="56"/>
-      <c r="K188" s="47"/>
-      <c r="L188" s="57"/>
-      <c r="M188" s="58"/>
-      <c r="N188" s="57"/>
-      <c r="O188" s="47"/>
-    </row>
-    <row r="189" ht="23" customHeight="1" spans="1:15">
-      <c r="A189" s="30"/>
-      <c r="B189" s="35"/>
-      <c r="C189" s="36"/>
-      <c r="D189" s="37"/>
-      <c r="E189" s="37"/>
-      <c r="F189" s="37"/>
-      <c r="G189" s="37"/>
-      <c r="H189" s="37"/>
-      <c r="I189" s="37"/>
-      <c r="J189" s="56"/>
-      <c r="K189" s="47"/>
-      <c r="L189" s="57"/>
-      <c r="M189" s="58"/>
-      <c r="N189" s="57"/>
-      <c r="O189" s="47"/>
-    </row>
-    <row r="190" ht="23" customHeight="1" spans="1:15">
-      <c r="A190" s="30"/>
-      <c r="B190" s="35"/>
-      <c r="C190" s="36"/>
-      <c r="D190" s="37"/>
-      <c r="E190" s="37"/>
-      <c r="F190" s="37"/>
-      <c r="G190" s="37"/>
-      <c r="H190" s="37"/>
-      <c r="I190" s="37"/>
-      <c r="J190" s="56"/>
-      <c r="K190" s="47"/>
-      <c r="L190" s="57"/>
-      <c r="M190" s="58"/>
-      <c r="N190" s="57"/>
-      <c r="O190" s="47"/>
-    </row>
   </sheetData>
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0"/>
   <mergeCells count="4">
@@ -17492,17 +15862,6 @@
       <formula>LEFT(N99,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N121:N190">
-    <cfRule type="beginsWith" dxfId="2" priority="370" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N121,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="371" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N121,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="372" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N121,LEN("PASS"))="PASS"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="N25:N27 N31">
     <cfRule type="beginsWith" dxfId="2" priority="13" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N25,LEN("WARN"))="WARN"</formula>
@@ -17570,10 +15929,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C12 C32 C33 C34 C37 C40 C41 C42 C43 C44 C46 C47 C48 C49 C50 C51 C52 C53 C54 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C69 C70 C71 C72 C73 C74 C75 C76 C77 C78 C79 C80 C81 C82 C83 C84 C85 C86 C87 C88 C89 C90 C91 C92 C93 C94 C95 C96 C97 C98 C99 C100 C101 C102 C103 C104 C105 C106 C107 C108 C109 C110 C111 C112 C113 C114 C115 C116 C117 C118 C119 C120 C13:C14 C35:C36 C38:C39 C121:C190">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C12 C32 C33 C34 C37 C40 C41 C42 C43 C44 C46 C47 C48 C49 C50 C51 C52 C53 C54 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C69 C70 C71 C72 C73 C74 C75 C76 C77 C78 C79 C80 C81 C82 C83 C84 C85 C86 C87 C88 C89 C90 C91 C92 C93 C94 C95 C96 C97 C98 C99 C100 C101 C102 C103 C104 C105 C106 C107 C108 C109 C110 C111 C112 C113 C114 C115 C116 C117 C118 C119 C120 C13:C14 C35:C36 C38:C39">
       <formula1>target</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D8 D9 D10 D11 D12 D17 D32 D33 D34 D37 D42 D43 D44 D46 D47 D48 D49 D50 D51 D52 D53 D54 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D71 D72 D73 D74 D75 D76 D77 D78 D79 D80 D81 D82 D83 D84 D85 D86 D87 D88 D89 D90 D91 D92 D93 D94 D95 D96 D97 D98 D99 D100 D101 D102 D103 D104 D105 D106 D107 D108 D109 D110 D111 D112 D113 D114 D115 D116 D117 D118 D119 D120 D13:D14 D35:D36 D38:D39 D40:D41 D121:D190">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D8 D9 D10 D11 D12 D17 D32 D33 D34 D37 D42 D43 D44 D46 D47 D48 D49 D50 D51 D52 D53 D54 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D71 D72 D73 D74 D75 D76 D77 D78 D79 D80 D81 D82 D83 D84 D85 D86 D87 D88 D89 D90 D91 D92 D93 D94 D95 D96 D97 D98 D99 D100 D101 D102 D103 D104 D105 D106 D107 D108 D109 D110 D111 D112 D113 D114 D115 D116 D117 D118 D119 D120 D13:D14 D35:D36 D38:D39 D40:D41">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>
@@ -17585,12 +15944,12 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O153"/>
+  <dimension ref="A1:O132"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B59" sqref="B59"/>
+      <selection pane="bottomLeft" activeCell="A133" sqref="$A133:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
@@ -21054,363 +19413,6 @@
       <c r="N132" s="57"/>
       <c r="O132" s="47"/>
     </row>
-    <row r="133" ht="23" customHeight="1" spans="1:15">
-      <c r="A133" s="30"/>
-      <c r="B133" s="35"/>
-      <c r="C133" s="36"/>
-      <c r="D133" s="37"/>
-      <c r="E133" s="37"/>
-      <c r="F133" s="37"/>
-      <c r="G133" s="37"/>
-      <c r="H133" s="37"/>
-      <c r="I133" s="37"/>
-      <c r="J133" s="56"/>
-      <c r="K133" s="47"/>
-      <c r="L133" s="57"/>
-      <c r="M133" s="58"/>
-      <c r="N133" s="57"/>
-      <c r="O133" s="47"/>
-    </row>
-    <row r="134" ht="23" customHeight="1" spans="1:15">
-      <c r="A134" s="30"/>
-      <c r="B134" s="35"/>
-      <c r="C134" s="36"/>
-      <c r="D134" s="37"/>
-      <c r="E134" s="37"/>
-      <c r="F134" s="37"/>
-      <c r="G134" s="37"/>
-      <c r="H134" s="37"/>
-      <c r="I134" s="37"/>
-      <c r="J134" s="56"/>
-      <c r="K134" s="47"/>
-      <c r="L134" s="57"/>
-      <c r="M134" s="58"/>
-      <c r="N134" s="57"/>
-      <c r="O134" s="47"/>
-    </row>
-    <row r="135" ht="23" customHeight="1" spans="1:15">
-      <c r="A135" s="30"/>
-      <c r="B135" s="35"/>
-      <c r="C135" s="36"/>
-      <c r="D135" s="37"/>
-      <c r="E135" s="37"/>
-      <c r="F135" s="37"/>
-      <c r="G135" s="37"/>
-      <c r="H135" s="37"/>
-      <c r="I135" s="37"/>
-      <c r="J135" s="56"/>
-      <c r="K135" s="47"/>
-      <c r="L135" s="57"/>
-      <c r="M135" s="58"/>
-      <c r="N135" s="57"/>
-      <c r="O135" s="47"/>
-    </row>
-    <row r="136" ht="23" customHeight="1" spans="1:15">
-      <c r="A136" s="30"/>
-      <c r="B136" s="35"/>
-      <c r="C136" s="36"/>
-      <c r="D136" s="37"/>
-      <c r="E136" s="37"/>
-      <c r="F136" s="37"/>
-      <c r="G136" s="37"/>
-      <c r="H136" s="37"/>
-      <c r="I136" s="37"/>
-      <c r="J136" s="56"/>
-      <c r="K136" s="47"/>
-      <c r="L136" s="57"/>
-      <c r="M136" s="58"/>
-      <c r="N136" s="57"/>
-      <c r="O136" s="47"/>
-    </row>
-    <row r="137" ht="23" customHeight="1" spans="1:15">
-      <c r="A137" s="30"/>
-      <c r="B137" s="35"/>
-      <c r="C137" s="36"/>
-      <c r="D137" s="37"/>
-      <c r="E137" s="37"/>
-      <c r="F137" s="37"/>
-      <c r="G137" s="37"/>
-      <c r="H137" s="37"/>
-      <c r="I137" s="37"/>
-      <c r="J137" s="56"/>
-      <c r="K137" s="47"/>
-      <c r="L137" s="57"/>
-      <c r="M137" s="58"/>
-      <c r="N137" s="57"/>
-      <c r="O137" s="47"/>
-    </row>
-    <row r="138" ht="23" customHeight="1" spans="1:15">
-      <c r="A138" s="30"/>
-      <c r="B138" s="35"/>
-      <c r="C138" s="36"/>
-      <c r="D138" s="37"/>
-      <c r="E138" s="37"/>
-      <c r="F138" s="37"/>
-      <c r="G138" s="37"/>
-      <c r="H138" s="37"/>
-      <c r="I138" s="37"/>
-      <c r="J138" s="56"/>
-      <c r="K138" s="47"/>
-      <c r="L138" s="57"/>
-      <c r="M138" s="58"/>
-      <c r="N138" s="57"/>
-      <c r="O138" s="47"/>
-    </row>
-    <row r="139" ht="23" customHeight="1" spans="1:15">
-      <c r="A139" s="30"/>
-      <c r="B139" s="35"/>
-      <c r="C139" s="36"/>
-      <c r="D139" s="37"/>
-      <c r="E139" s="37"/>
-      <c r="F139" s="37"/>
-      <c r="G139" s="37"/>
-      <c r="H139" s="37"/>
-      <c r="I139" s="37"/>
-      <c r="J139" s="56"/>
-      <c r="K139" s="47"/>
-      <c r="L139" s="57"/>
-      <c r="M139" s="58"/>
-      <c r="N139" s="57"/>
-      <c r="O139" s="47"/>
-    </row>
-    <row r="140" ht="23" customHeight="1" spans="1:15">
-      <c r="A140" s="30"/>
-      <c r="B140" s="35"/>
-      <c r="C140" s="36"/>
-      <c r="D140" s="37"/>
-      <c r="E140" s="37"/>
-      <c r="F140" s="37"/>
-      <c r="G140" s="37"/>
-      <c r="H140" s="37"/>
-      <c r="I140" s="37"/>
-      <c r="J140" s="56"/>
-      <c r="K140" s="47"/>
-      <c r="L140" s="57"/>
-      <c r="M140" s="58"/>
-      <c r="N140" s="57"/>
-      <c r="O140" s="47"/>
-    </row>
-    <row r="141" ht="23" customHeight="1" spans="1:15">
-      <c r="A141" s="30"/>
-      <c r="B141" s="35"/>
-      <c r="C141" s="36"/>
-      <c r="D141" s="37"/>
-      <c r="E141" s="37"/>
-      <c r="F141" s="37"/>
-      <c r="G141" s="37"/>
-      <c r="H141" s="37"/>
-      <c r="I141" s="37"/>
-      <c r="J141" s="56"/>
-      <c r="K141" s="47"/>
-      <c r="L141" s="57"/>
-      <c r="M141" s="58"/>
-      <c r="N141" s="57"/>
-      <c r="O141" s="47"/>
-    </row>
-    <row r="142" ht="23" customHeight="1" spans="1:15">
-      <c r="A142" s="30"/>
-      <c r="B142" s="35"/>
-      <c r="C142" s="36"/>
-      <c r="D142" s="37"/>
-      <c r="E142" s="37"/>
-      <c r="F142" s="37"/>
-      <c r="G142" s="37"/>
-      <c r="H142" s="37"/>
-      <c r="I142" s="37"/>
-      <c r="J142" s="56"/>
-      <c r="K142" s="47"/>
-      <c r="L142" s="57"/>
-      <c r="M142" s="58"/>
-      <c r="N142" s="57"/>
-      <c r="O142" s="47"/>
-    </row>
-    <row r="143" ht="23" customHeight="1" spans="1:15">
-      <c r="A143" s="30"/>
-      <c r="B143" s="35"/>
-      <c r="C143" s="36"/>
-      <c r="D143" s="37"/>
-      <c r="E143" s="37"/>
-      <c r="F143" s="37"/>
-      <c r="G143" s="37"/>
-      <c r="H143" s="37"/>
-      <c r="I143" s="37"/>
-      <c r="J143" s="56"/>
-      <c r="K143" s="47"/>
-      <c r="L143" s="57"/>
-      <c r="M143" s="58"/>
-      <c r="N143" s="57"/>
-      <c r="O143" s="47"/>
-    </row>
-    <row r="144" ht="23" customHeight="1" spans="1:15">
-      <c r="A144" s="30"/>
-      <c r="B144" s="35"/>
-      <c r="C144" s="36"/>
-      <c r="D144" s="37"/>
-      <c r="E144" s="37"/>
-      <c r="F144" s="37"/>
-      <c r="G144" s="37"/>
-      <c r="H144" s="37"/>
-      <c r="I144" s="37"/>
-      <c r="J144" s="56"/>
-      <c r="K144" s="47"/>
-      <c r="L144" s="57"/>
-      <c r="M144" s="58"/>
-      <c r="N144" s="57"/>
-      <c r="O144" s="47"/>
-    </row>
-    <row r="145" ht="23" customHeight="1" spans="1:15">
-      <c r="A145" s="30"/>
-      <c r="B145" s="35"/>
-      <c r="C145" s="36"/>
-      <c r="D145" s="37"/>
-      <c r="E145" s="37"/>
-      <c r="F145" s="37"/>
-      <c r="G145" s="37"/>
-      <c r="H145" s="37"/>
-      <c r="I145" s="37"/>
-      <c r="J145" s="56"/>
-      <c r="K145" s="47"/>
-      <c r="L145" s="57"/>
-      <c r="M145" s="58"/>
-      <c r="N145" s="57"/>
-      <c r="O145" s="47"/>
-    </row>
-    <row r="146" ht="23" customHeight="1" spans="1:15">
-      <c r="A146" s="30"/>
-      <c r="B146" s="35"/>
-      <c r="C146" s="36"/>
-      <c r="D146" s="37"/>
-      <c r="E146" s="37"/>
-      <c r="F146" s="37"/>
-      <c r="G146" s="37"/>
-      <c r="H146" s="37"/>
-      <c r="I146" s="37"/>
-      <c r="J146" s="56"/>
-      <c r="K146" s="47"/>
-      <c r="L146" s="57"/>
-      <c r="M146" s="58"/>
-      <c r="N146" s="57"/>
-      <c r="O146" s="47"/>
-    </row>
-    <row r="147" ht="23" customHeight="1" spans="1:15">
-      <c r="A147" s="30"/>
-      <c r="B147" s="35"/>
-      <c r="C147" s="36"/>
-      <c r="D147" s="37"/>
-      <c r="E147" s="37"/>
-      <c r="F147" s="37"/>
-      <c r="G147" s="37"/>
-      <c r="H147" s="37"/>
-      <c r="I147" s="37"/>
-      <c r="J147" s="56"/>
-      <c r="K147" s="47"/>
-      <c r="L147" s="57"/>
-      <c r="M147" s="58"/>
-      <c r="N147" s="57"/>
-      <c r="O147" s="47"/>
-    </row>
-    <row r="148" ht="23" customHeight="1" spans="1:15">
-      <c r="A148" s="30"/>
-      <c r="B148" s="35"/>
-      <c r="C148" s="36"/>
-      <c r="D148" s="37"/>
-      <c r="E148" s="37"/>
-      <c r="F148" s="37"/>
-      <c r="G148" s="37"/>
-      <c r="H148" s="37"/>
-      <c r="I148" s="37"/>
-      <c r="J148" s="56"/>
-      <c r="K148" s="47"/>
-      <c r="L148" s="57"/>
-      <c r="M148" s="58"/>
-      <c r="N148" s="57"/>
-      <c r="O148" s="47"/>
-    </row>
-    <row r="149" ht="23" customHeight="1" spans="1:15">
-      <c r="A149" s="30"/>
-      <c r="B149" s="35"/>
-      <c r="C149" s="36"/>
-      <c r="D149" s="37"/>
-      <c r="E149" s="37"/>
-      <c r="F149" s="37"/>
-      <c r="G149" s="37"/>
-      <c r="H149" s="37"/>
-      <c r="I149" s="37"/>
-      <c r="J149" s="56"/>
-      <c r="K149" s="47"/>
-      <c r="L149" s="57"/>
-      <c r="M149" s="58"/>
-      <c r="N149" s="57"/>
-      <c r="O149" s="47"/>
-    </row>
-    <row r="150" ht="23" customHeight="1" spans="1:15">
-      <c r="A150" s="30"/>
-      <c r="B150" s="35"/>
-      <c r="C150" s="36"/>
-      <c r="D150" s="37"/>
-      <c r="E150" s="37"/>
-      <c r="F150" s="37"/>
-      <c r="G150" s="37"/>
-      <c r="H150" s="37"/>
-      <c r="I150" s="37"/>
-      <c r="J150" s="56"/>
-      <c r="K150" s="47"/>
-      <c r="L150" s="57"/>
-      <c r="M150" s="58"/>
-      <c r="N150" s="57"/>
-      <c r="O150" s="47"/>
-    </row>
-    <row r="151" ht="23" customHeight="1" spans="1:15">
-      <c r="A151" s="30"/>
-      <c r="B151" s="35"/>
-      <c r="C151" s="36"/>
-      <c r="D151" s="37"/>
-      <c r="E151" s="37"/>
-      <c r="F151" s="37"/>
-      <c r="G151" s="37"/>
-      <c r="H151" s="37"/>
-      <c r="I151" s="37"/>
-      <c r="J151" s="56"/>
-      <c r="K151" s="47"/>
-      <c r="L151" s="57"/>
-      <c r="M151" s="58"/>
-      <c r="N151" s="57"/>
-      <c r="O151" s="47"/>
-    </row>
-    <row r="152" ht="23" customHeight="1" spans="1:15">
-      <c r="A152" s="30"/>
-      <c r="B152" s="35"/>
-      <c r="C152" s="36"/>
-      <c r="D152" s="37"/>
-      <c r="E152" s="37"/>
-      <c r="F152" s="37"/>
-      <c r="G152" s="37"/>
-      <c r="H152" s="37"/>
-      <c r="I152" s="37"/>
-      <c r="J152" s="56"/>
-      <c r="K152" s="47"/>
-      <c r="L152" s="57"/>
-      <c r="M152" s="58"/>
-      <c r="N152" s="57"/>
-      <c r="O152" s="47"/>
-    </row>
-    <row r="153" ht="23" customHeight="1" spans="1:15">
-      <c r="A153" s="30"/>
-      <c r="B153" s="35"/>
-      <c r="C153" s="36"/>
-      <c r="D153" s="37"/>
-      <c r="E153" s="37"/>
-      <c r="F153" s="37"/>
-      <c r="G153" s="37"/>
-      <c r="H153" s="37"/>
-      <c r="I153" s="37"/>
-      <c r="J153" s="56"/>
-      <c r="K153" s="47"/>
-      <c r="L153" s="57"/>
-      <c r="M153" s="58"/>
-      <c r="N153" s="57"/>
-      <c r="O153" s="47"/>
-    </row>
   </sheetData>
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0"/>
   <mergeCells count="4">
@@ -22057,17 +20059,6 @@
       <formula>LEFT(N106,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N133:N153">
-    <cfRule type="beginsWith" dxfId="2" priority="385" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N133,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="386" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N133,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="387" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N133,LEN("PASS"))="PASS"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="N22:N24 N55:N57 N26">
     <cfRule type="beginsWith" dxfId="2" priority="223" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N22,LEN("WARN"))="WARN"</formula>
@@ -22146,10 +20137,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C27 C28 C29 C30 C33 C34 C35 C36 C37 C38 C39 C40 C41 C42 C43 C46 C47 C48 C50 C51 C52 C53 C54 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C69 C70 C71 C72 C73 C74 C75 C76 C77 C78 C79 C80 C81 C82 C83 C84 C85 C86 C87 C88 C89 C90 C91 C92 C93 C94 C95 C96 C97 C98 C99 C100 C101 C102 C103 C104 C105 C106 C107 C108 C109 C110 C111 C112 C113 C114 C115 C116 C117 C118 C119 C120 C121 C122 C123 C124 C125 C126 C127 C128 C129 C130 C131 C132 C11:C12 C31:C32 C44:C45 C133:C153">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C27 C28 C29 C30 C33 C34 C35 C36 C37 C38 C39 C40 C41 C42 C43 C46 C47 C48 C50 C51 C52 C53 C54 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C69 C70 C71 C72 C73 C74 C75 C76 C77 C78 C79 C80 C81 C82 C83 C84 C85 C86 C87 C88 C89 C90 C91 C92 C93 C94 C95 C96 C97 C98 C99 C100 C101 C102 C103 C104 C105 C106 C107 C108 C109 C110 C111 C112 C113 C114 C115 C116 C117 C118 C119 C120 C121 C122 C123 C124 C125 C126 C127 C128 C129 C130 C131 C132 C11:C12 C31:C32 C44:C45">
       <formula1>target</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D8 D9 D10 D15 D22 D27 D28 D29 D30 D35 D36 D37 D38 D39 D40 D41 D42 D43 D46 D47 D48 D50 D51 D52 D53 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D71 D72 D73 D74 D75 D76 D77 D78 D79 D80 D81 D82 D83 D84 D85 D86 D87 D88 D89 D90 D91 D92 D93 D94 D95 D96 D97 D98 D99 D100 D101 D102 D103 D104 D105 D106 D107 D108 D109 D110 D111 D112 D113 D114 D115 D116 D117 D118 D119 D120 D121 D122 D123 D124 D125 D126 D127 D128 D129 D130 D131 D132 D11:D12 D23:D26 D31:D32 D33:D34 D44:D45 D133:D153">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D8 D9 D10 D15 D22 D27 D28 D29 D30 D35 D36 D37 D38 D39 D40 D41 D42 D43 D46 D47 D48 D50 D51 D52 D53 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D71 D72 D73 D74 D75 D76 D77 D78 D79 D80 D81 D82 D83 D84 D85 D86 D87 D88 D89 D90 D91 D92 D93 D94 D95 D96 D97 D98 D99 D100 D101 D102 D103 D104 D105 D106 D107 D108 D109 D110 D111 D112 D113 D114 D115 D116 D117 D118 D119 D120 D121 D122 D123 D124 D125 D126 D127 D128 D129 D130 D131 D132 D11:D12 D23:D26 D31:D32 D33:D34 D44:D45">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>
@@ -22161,12 +20152,12 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O164"/>
+  <dimension ref="A1:O157"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
+      <selection pane="bottomLeft" activeCell="E179" sqref="E179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
@@ -26324,125 +24315,6 @@
       <c r="N157" s="57"/>
       <c r="O157" s="47"/>
     </row>
-    <row r="158" ht="23" customHeight="1" spans="1:15">
-      <c r="A158" s="30"/>
-      <c r="B158" s="35"/>
-      <c r="C158" s="36"/>
-      <c r="D158" s="37"/>
-      <c r="E158" s="37"/>
-      <c r="F158" s="37"/>
-      <c r="G158" s="37"/>
-      <c r="H158" s="37"/>
-      <c r="I158" s="37"/>
-      <c r="J158" s="56"/>
-      <c r="K158" s="47"/>
-      <c r="L158" s="57"/>
-      <c r="M158" s="58"/>
-      <c r="N158" s="57"/>
-      <c r="O158" s="47"/>
-    </row>
-    <row r="159" ht="23" customHeight="1" spans="1:15">
-      <c r="A159" s="30"/>
-      <c r="B159" s="35"/>
-      <c r="C159" s="36"/>
-      <c r="D159" s="37"/>
-      <c r="E159" s="37"/>
-      <c r="F159" s="37"/>
-      <c r="G159" s="37"/>
-      <c r="H159" s="37"/>
-      <c r="I159" s="37"/>
-      <c r="J159" s="56"/>
-      <c r="K159" s="47"/>
-      <c r="L159" s="57"/>
-      <c r="M159" s="58"/>
-      <c r="N159" s="57"/>
-      <c r="O159" s="47"/>
-    </row>
-    <row r="160" ht="23" customHeight="1" spans="1:15">
-      <c r="A160" s="30"/>
-      <c r="B160" s="35"/>
-      <c r="C160" s="36"/>
-      <c r="D160" s="37"/>
-      <c r="E160" s="37"/>
-      <c r="F160" s="37"/>
-      <c r="G160" s="37"/>
-      <c r="H160" s="37"/>
-      <c r="I160" s="37"/>
-      <c r="J160" s="56"/>
-      <c r="K160" s="47"/>
-      <c r="L160" s="57"/>
-      <c r="M160" s="58"/>
-      <c r="N160" s="57"/>
-      <c r="O160" s="47"/>
-    </row>
-    <row r="161" ht="23" customHeight="1" spans="1:15">
-      <c r="A161" s="30"/>
-      <c r="B161" s="35"/>
-      <c r="C161" s="36"/>
-      <c r="D161" s="37"/>
-      <c r="E161" s="37"/>
-      <c r="F161" s="37"/>
-      <c r="G161" s="37"/>
-      <c r="H161" s="37"/>
-      <c r="I161" s="37"/>
-      <c r="J161" s="56"/>
-      <c r="K161" s="47"/>
-      <c r="L161" s="57"/>
-      <c r="M161" s="58"/>
-      <c r="N161" s="57"/>
-      <c r="O161" s="47"/>
-    </row>
-    <row r="162" ht="23" customHeight="1" spans="1:15">
-      <c r="A162" s="30"/>
-      <c r="B162" s="35"/>
-      <c r="C162" s="36"/>
-      <c r="D162" s="37"/>
-      <c r="E162" s="37"/>
-      <c r="F162" s="37"/>
-      <c r="G162" s="37"/>
-      <c r="H162" s="37"/>
-      <c r="I162" s="37"/>
-      <c r="J162" s="56"/>
-      <c r="K162" s="47"/>
-      <c r="L162" s="57"/>
-      <c r="M162" s="58"/>
-      <c r="N162" s="57"/>
-      <c r="O162" s="47"/>
-    </row>
-    <row r="163" ht="23" customHeight="1" spans="1:15">
-      <c r="A163" s="30"/>
-      <c r="B163" s="35"/>
-      <c r="C163" s="36"/>
-      <c r="D163" s="37"/>
-      <c r="E163" s="37"/>
-      <c r="F163" s="37"/>
-      <c r="G163" s="37"/>
-      <c r="H163" s="37"/>
-      <c r="I163" s="37"/>
-      <c r="J163" s="56"/>
-      <c r="K163" s="47"/>
-      <c r="L163" s="57"/>
-      <c r="M163" s="58"/>
-      <c r="N163" s="57"/>
-      <c r="O163" s="47"/>
-    </row>
-    <row r="164" ht="23" customHeight="1" spans="1:15">
-      <c r="A164" s="30"/>
-      <c r="B164" s="35"/>
-      <c r="C164" s="36"/>
-      <c r="D164" s="37"/>
-      <c r="E164" s="37"/>
-      <c r="F164" s="37"/>
-      <c r="G164" s="37"/>
-      <c r="H164" s="37"/>
-      <c r="I164" s="37"/>
-      <c r="J164" s="56"/>
-      <c r="K164" s="47"/>
-      <c r="L164" s="57"/>
-      <c r="M164" s="58"/>
-      <c r="N164" s="57"/>
-      <c r="O164" s="47"/>
-    </row>
   </sheetData>
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0"/>
   <mergeCells count="4">
@@ -27177,7 +25049,7 @@
       <formula>LEFT(N156,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N8:N11 N158:N164 N15:N16">
+  <conditionalFormatting sqref="N8:N11 N15:N16">
     <cfRule type="beginsWith" dxfId="2" priority="298" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N8,LEN("WARN"))="WARN"</formula>
     </cfRule>
@@ -27277,10 +25149,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C10 C11 C12 C13 C14 C17 C18 C19 C20 C21 C22 C23 C24 C25 C26 C27 C28 C29 C30 C31 C32 C51 C52 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C71 C72 C73 C75 C76 C77 C78 C79 C80 C81 C82 C83 C84 C85 C86 C87 C88 C89 C90 C91 C92 C93 C94 C95 C96 C97 C98 C99 C100 C101 C102 C103 C104 C105 C106 C107 C108 C109 C110 C111 C112 C113 C114 C115 C116 C117 C118 C119 C120 C121 C122 C123 C124 C125 C126 C127 C128 C129 C130 C131 C132 C133 C134 C135 C136 C137 C138 C139 C140 C141 C142 C143 C144 C145 C146 C147 C148 C149 C150 C151 C152 C153 C154 C155 C156 C157 C8:C9 C15:C16 C33:C34 C53:C54 C69:C70 C158:C164">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C10 C11 C12 C13 C14 C17 C18 C19 C20 C21 C22 C23 C24 C25 C26 C27 C28 C29 C30 C31 C32 C51 C52 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C71 C72 C73 C75 C76 C77 C78 C79 C80 C81 C82 C83 C84 C85 C86 C87 C88 C89 C90 C91 C92 C93 C94 C95 C96 C97 C98 C99 C100 C101 C102 C103 C104 C105 C106 C107 C108 C109 C110 C111 C112 C113 C114 C115 C116 C117 C118 C119 C120 C121 C122 C123 C124 C125 C126 C127 C128 C129 C130 C131 C132 C133 C134 C135 C136 C137 C138 C139 C140 C141 C142 C143 C144 C145 C146 C147 C148 C149 C150 C151 C152 C153 C154 C155 C156 C157 C8:C9 C15:C16 C33:C34 C53:C54 C69:C70">
       <formula1>target</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D37 D44 D48 D49 D50 D51 D52 D53 D54 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D71 D72 D73 D75 D76 D77 D78 D80 D81 D82 D83 D84 D85 D86 D87 D88 D89 D90 D91 D92 D93 D94 D95 D96 D97 D98 D99 D100 D101 D102 D103 D104 D105 D106 D107 D108 D109 D110 D111 D112 D113 D114 D115 D116 D117 D118 D119 D120 D121 D122 D123 D124 D125 D126 D127 D128 D129 D130 D131 D132 D133 D134 D135 D136 D137 D138 D139 D140 D141 D142 D143 D144 D145 D146 D147 D148 D149 D150 D151 D152 D153 D154 D155 D156 D157 D8:D9 D33:D34 D45:D47 D69:D70 D158:D164">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D37 D44 D48 D49 D50 D51 D52 D53 D54 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D71 D72 D73 D75 D76 D77 D78 D80 D81 D82 D83 D84 D85 D86 D87 D88 D89 D90 D91 D92 D93 D94 D95 D96 D97 D98 D99 D100 D101 D102 D103 D104 D105 D106 D107 D108 D109 D110 D111 D112 D113 D114 D115 D116 D117 D118 D119 D120 D121 D122 D123 D124 D125 D126 D127 D128 D129 D130 D131 D132 D133 D134 D135 D136 D137 D138 D139 D140 D141 D142 D143 D144 D145 D146 D147 D148 D149 D150 D151 D152 D153 D154 D155 D156 D157 D8:D9 D33:D34 D45:D47 D69:D70">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>